<commit_message>
[WIP] working on producing result
</commit_message>
<xml_diff>
--- a/example/DeliveryList_2.xlsx
+++ b/example/DeliveryList_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
   <si>
     <t xml:space="preserve">번호</t>
   </si>
@@ -227,6 +227,66 @@
   </si>
   <si>
     <t xml:space="preserve">판매자 배송</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5739885993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32100020883943</t>
+  </si>
+  <si>
+    <t xml:space="preserve">우체국</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6094321250183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-08 15:39:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-11-25 11:10:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">베이비뵨 바운서 밸런스 소프트 메쉬 스카이 블루</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6720117486</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82844419727</t>
+  </si>
+  <si>
+    <t xml:space="preserve">베이비뵨 바운서 밸런스 소프트 메쉬 스카이 블루,단일상품</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8434555784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">한규택</t>
+  </si>
+  <si>
+    <t xml:space="preserve">010-****-****</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Han Seungho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13596</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-09 19:43:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-16 20:10:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P210023276057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">010-5253-6534</t>
   </si>
 </sst>
 </file>
@@ -248,19 +308,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="129"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="129"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="129"/>
     </font>
   </fonts>
   <fills count="3">
@@ -323,11 +380,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,10 +405,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.8359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -581,6 +638,116 @@
         <v>67</v>
       </c>
       <c r="AN2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN3" s="2" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>